<commit_message>
exception proofing the scraper
</commit_message>
<xml_diff>
--- a/static/test.xlsx
+++ b/static/test.xlsx
@@ -14,47 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
-  <si>
-    <t>ANZ Advanced</t>
-  </si>
-  <si>
-    <t>CBA</t>
-  </si>
-  <si>
-    <t>Westpac</t>
-  </si>
-  <si>
-    <t>NAB</t>
-  </si>
-  <si>
-    <t>St George</t>
-  </si>
-  <si>
-    <t>Bankwest</t>
-  </si>
-  <si>
-    <t>UBank standard rate</t>
-  </si>
-  <si>
-    <t>BOQ</t>
-  </si>
-  <si>
-    <t>Citibank</t>
-  </si>
-  <si>
-    <t>30/01/2017</t>
-  </si>
-  <si>
-    <t>Short term</t>
-  </si>
-  <si>
-    <t>Mid term</t>
-  </si>
-  <si>
-    <t>Long term</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,215 +348,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:29">
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" t="s">
-        <v>6</v>
-      </c>
-      <c r="X1" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="n">
-        <v>90</v>
-      </c>
-      <c r="D2" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="F2" t="n">
-        <v>90</v>
-      </c>
-      <c r="G2" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="I2" t="n">
-        <v>90</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>90</v>
-      </c>
-      <c r="M2" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>90</v>
-      </c>
-      <c r="P2" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="R2" t="n">
-        <v>90</v>
-      </c>
-      <c r="S2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="U2" t="n">
-        <v>90</v>
-      </c>
-      <c r="V2" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="X2" t="n">
-        <v>90</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29">
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="n">
-        <v>120</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="F3" t="n">
-        <v>210</v>
-      </c>
-      <c r="G3" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="I3" t="n">
-        <v>180</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="L3" t="n">
-        <v>240</v>
-      </c>
-      <c r="M3" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="O3" t="n">
-        <v>180</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="R3" t="n">
-        <v>210</v>
-      </c>
-      <c r="S3" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="U3" t="n">
-        <v>180</v>
-      </c>
-      <c r="V3" t="n">
-        <v>2.61</v>
-      </c>
-      <c r="X3" t="n">
-        <v>180</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="n">
-        <v>360</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2.55</v>
-      </c>
-      <c r="F4" t="n">
-        <v>360</v>
-      </c>
-      <c r="G4" t="n">
-        <v>2.35</v>
-      </c>
-      <c r="I4" t="n">
-        <v>360</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="L4" t="n">
-        <v>360</v>
-      </c>
-      <c r="M4" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="O4" t="n">
-        <v>360</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="R4" t="n">
-        <v>360</v>
-      </c>
-      <c r="S4" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="U4" t="n">
-        <v>360</v>
-      </c>
-      <c r="V4" t="n">
-        <v>2.71</v>
-      </c>
-      <c r="X4" t="n">
-        <v>360</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>360</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
widget bar for TD added
</commit_message>
<xml_diff>
--- a/static/test.xlsx
+++ b/static/test.xlsx
@@ -14,7 +14,47 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+  <si>
+    <t>ANZ Standard</t>
+  </si>
+  <si>
+    <t>ANZ Advanced</t>
+  </si>
+  <si>
+    <t>CBA</t>
+  </si>
+  <si>
+    <t>Westpac</t>
+  </si>
+  <si>
+    <t>NAB</t>
+  </si>
+  <si>
+    <t>St George</t>
+  </si>
+  <si>
+    <t>Bankwest</t>
+  </si>
+  <si>
+    <t>UBank Loyalty Bonus</t>
+  </si>
+  <si>
+    <t>Citibank</t>
+  </si>
+  <si>
+    <t>2017-02-19 21:50:48.032549</t>
+  </si>
+  <si>
+    <t>Short term</t>
+  </si>
+  <si>
+    <t>Mid term</t>
+  </si>
+  <si>
+    <t>Long term</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -348,14 +388,215 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="n">
+        <v>90</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>90</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>90</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="L2" t="n">
+        <v>90</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="O2" t="n">
+        <v>90</v>
+      </c>
+      <c r="P2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>90</v>
+      </c>
+      <c r="S2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>90</v>
+      </c>
+      <c r="V2" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="X2" t="n">
+        <v>90</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="n">
+        <v>180</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>120</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>210</v>
+      </c>
+      <c r="J3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>180</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>240</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="R3" t="n">
+        <v>180</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="U3" t="n">
+        <v>210</v>
+      </c>
+      <c r="V3" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="X3" t="n">
+        <v>180</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="n">
+        <v>360</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="F4" t="n">
+        <v>360</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="I4" t="n">
+        <v>360</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="L4" t="n">
+        <v>360</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="O4" t="n">
+        <v>360</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="R4" t="n">
+        <v>360</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="U4" t="n">
+        <v>360</v>
+      </c>
+      <c r="V4" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="X4" t="n">
+        <v>360</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>360</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>